<commit_message>
Added transportation costs to feedstock costs.
</commit_message>
<xml_diff>
--- a/examples/H2_Analysis/green_steel_site_renewable_costs_ATB.xlsx
+++ b/examples/H2_Analysis/green_steel_site_renewable_costs_ATB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jannoni/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kbrunik/github/HOPP/examples/H2_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630BA928-6235-A646-86E4-53E1AB1BF57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F17E7D-9792-1841-8962-2AFFAEDB8ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11100" yWindow="660" windowWidth="28800" windowHeight="17500" xr2:uid="{1FCD4B6C-D650-7B41-B236-554783F4AED6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{1FCD4B6C-D650-7B41-B236-554783F4AED6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>State</t>
   </si>
@@ -177,6 +177,15 @@
   </si>
   <si>
     <t>2035 PV OpEx</t>
+  </si>
+  <si>
+    <t>Lime Transport ($/metric tonne)</t>
+  </si>
+  <si>
+    <t>Carbon Transport ($/metric tonne)</t>
+  </si>
+  <si>
+    <t>Iron Ore Pellets Transport ($/metric tonne)</t>
   </si>
 </sst>
 </file>
@@ -228,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -241,6 +250,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49799FC5-21F5-FB4A-92B9-AD28EDE30D2D}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1125,16 +1135,16 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>155.34</v>
+        <v>100</v>
       </c>
       <c r="C35">
-        <v>141.51</v>
+        <v>100</v>
       </c>
       <c r="D35">
-        <v>155.34</v>
+        <v>100</v>
       </c>
       <c r="E35">
-        <v>169.18</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1142,16 +1152,16 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>218.74</v>
+        <v>190</v>
       </c>
       <c r="C36">
-        <v>264.94</v>
+        <v>190</v>
       </c>
       <c r="D36">
-        <v>229.74</v>
+        <v>190</v>
       </c>
       <c r="E36">
-        <v>245.14</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1159,16 +1169,67 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>230.52</v>
+        <v>207</v>
       </c>
       <c r="C37">
-        <v>292.2</v>
+        <v>207</v>
       </c>
       <c r="D37">
-        <v>239.32</v>
+        <v>207</v>
       </c>
       <c r="E37">
-        <v>270.2</v>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="6">
+        <v>15.304355133142501</v>
+      </c>
+      <c r="C38" s="6">
+        <v>13.994888138197</v>
+      </c>
+      <c r="D38" s="6">
+        <v>15.6787156073425</v>
+      </c>
+      <c r="E38" s="6">
+        <v>24.278765187454798</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39">
+        <v>21.655389551229899</v>
+      </c>
+      <c r="C39">
+        <v>38.804157019719902</v>
+      </c>
+      <c r="D39">
+        <v>28.260162830812401</v>
+      </c>
+      <c r="E39">
+        <v>18.397699324604002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40">
+        <v>14.5240261890238</v>
+      </c>
+      <c r="C40">
+        <v>57.888084159733403</v>
+      </c>
+      <c r="D40">
+        <v>17.7384920497378</v>
+      </c>
+      <c r="E40">
+        <v>57.588434738181697</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Wyoming site. placeholder values: turbine cost, water cost, hydrogen storage type
</commit_message>
<xml_diff>
--- a/examples/H2_Analysis/green_steel_site_renewable_costs_ATB.xlsx
+++ b/examples/H2_Analysis/green_steel_site_renewable_costs_ATB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jannoni/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/egrant/Desktop/HOPP-GIT/HOPP/examples/H2_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630BA928-6235-A646-86E4-53E1AB1BF57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB84D91-63D8-FE45-919A-596A06C72486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11100" yWindow="660" windowWidth="28800" windowHeight="17500" xr2:uid="{1FCD4B6C-D650-7B41-B236-554783F4AED6}"/>
+    <workbookView xWindow="41160" yWindow="1120" windowWidth="28800" windowHeight="19440" xr2:uid="{1FCD4B6C-D650-7B41-B236-554783F4AED6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>State</t>
   </si>
@@ -134,9 +134,6 @@
     <t>41.62, -87.22</t>
   </si>
   <si>
-    <t>34.22, -102.75</t>
-  </si>
-  <si>
     <t>42.55, -90.69</t>
   </si>
   <si>
@@ -177,6 +174,27 @@
   </si>
   <si>
     <t>2035 PV OpEx</t>
+  </si>
+  <si>
+    <t>Site 5</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>41.659, -107.416</t>
+  </si>
+  <si>
+    <t>Lime Transport ($/metric tonne)</t>
+  </si>
+  <si>
+    <t>Carbon Transport ($/metric tonne)</t>
+  </si>
+  <si>
+    <t>Iron Ore Pellets Transport ($/metric tonne)</t>
+  </si>
+  <si>
+    <t>29.92,-100.647</t>
   </si>
 </sst>
 </file>
@@ -199,12 +217,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -228,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -241,6 +271,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49799FC5-21F5-FB4A-92B9-AD28EDE30D2D}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,7 +610,7 @@
     <col min="4" max="5" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -585,8 +626,11 @@
       <c r="E1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,33 +646,39 @@
       <c r="E2" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3">
         <v>41.62</v>
       </c>
-      <c r="C4" s="3">
-        <v>34.22</v>
+      <c r="C4" s="10">
+        <v>29.92</v>
       </c>
       <c r="D4" s="3">
         <v>42.55</v>
@@ -636,16 +686,19 @@
       <c r="E4" s="3">
         <v>30.45</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="3">
+        <v>41.658999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3">
         <v>-87.22</v>
       </c>
-      <c r="C5" s="3">
-        <v>-102.75</v>
+      <c r="C5" s="9">
+        <v>-100.64700000000001</v>
       </c>
       <c r="D5" s="3">
         <v>-90.69</v>
@@ -653,8 +706,11 @@
       <c r="E5" s="3">
         <v>-89.35</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="3">
+        <v>-107.416</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -670,8 +726,11 @@
       <c r="E6" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -687,8 +746,11 @@
       <c r="E7" s="3">
         <v>185</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -704,8 +766,11 @@
       <c r="E8" s="3">
         <v>130</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -721,10 +786,13 @@
       <c r="E9" s="3">
         <v>2232</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="3">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="3">
         <v>1210</v>
@@ -738,8 +806,11 @@
       <c r="E10" s="3">
         <v>1938</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="3">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -755,10 +826,13 @@
       <c r="E11" s="3">
         <v>1644</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="3">
         <v>985.5</v>
@@ -772,8 +846,11 @@
       <c r="E12" s="3">
         <v>1613</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="3">
+        <v>985.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -789,8 +866,11 @@
       <c r="E13" s="3">
         <v>1520</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="3">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -806,8 +886,11 @@
       <c r="E14" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -823,10 +906,13 @@
       <c r="E15" s="3">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="3">
         <v>38.69</v>
@@ -840,8 +926,11 @@
       <c r="E16" s="3">
         <v>38.69</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="3">
+        <v>38.69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -857,10 +946,13 @@
       <c r="E17" s="2">
         <v>34.380000000000003</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="2">
+        <v>34.380000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="2">
         <v>31.801500000000004</v>
@@ -874,8 +966,11 @@
       <c r="E18" s="2">
         <v>31.801500000000004</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="2">
+        <v>31.801500000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -891,8 +986,11 @@
       <c r="E19" s="2">
         <v>24.065999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="2">
+        <v>24.065999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -908,15 +1006,18 @@
       <c r="E20" s="2">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="2">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
@@ -932,10 +1033,13 @@
       <c r="E22" s="2">
         <v>1391</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="2">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2">
         <v>1014.3150000000001</v>
@@ -949,8 +1053,11 @@
       <c r="E23" s="2">
         <v>1014.3150000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="2">
+        <v>1014.3150000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
@@ -966,10 +1073,13 @@
       <c r="E24" s="2">
         <v>637.63</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="2">
+        <v>637.63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" s="2">
         <v>598.41999999999996</v>
@@ -983,10 +1093,13 @@
       <c r="E25" s="2">
         <v>598.41999999999996</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="2">
+        <v>598.41999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26">
         <v>480.79</v>
@@ -1000,8 +1113,11 @@
       <c r="E26">
         <v>480.79</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>480.79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>16</v>
       </c>
@@ -1017,8 +1133,11 @@
       <c r="E27">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>17</v>
       </c>
@@ -1034,10 +1153,13 @@
       <c r="E28">
         <v>22.62</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <v>22.62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29">
         <v>17.935000000000002</v>
@@ -1051,8 +1173,11 @@
       <c r="E29">
         <v>17.935000000000002</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <v>17.935000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -1068,10 +1193,13 @@
       <c r="E30">
         <v>13.25</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <v>13.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31">
         <v>12.6525</v>
@@ -1085,8 +1213,11 @@
       <c r="E31">
         <v>12.6525</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <v>12.6525</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -1102,8 +1233,11 @@
       <c r="E32">
         <v>10.86</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <v>10.86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -1119,56 +1253,128 @@
       <c r="E33">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>100</v>
+      </c>
+      <c r="C35">
+        <v>100</v>
+      </c>
+      <c r="D35">
+        <v>100</v>
+      </c>
+      <c r="E35">
+        <v>100</v>
+      </c>
+      <c r="F35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>35</v>
       </c>
-      <c r="B35">
-        <v>155.34</v>
-      </c>
-      <c r="C35">
-        <v>141.51</v>
-      </c>
-      <c r="D35">
-        <v>155.34</v>
-      </c>
-      <c r="E35">
-        <v>169.18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="B36">
+        <v>190</v>
+      </c>
+      <c r="C36">
+        <v>190</v>
+      </c>
+      <c r="D36">
+        <v>190</v>
+      </c>
+      <c r="E36">
+        <v>190</v>
+      </c>
+      <c r="F36">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="B36">
-        <v>218.74</v>
-      </c>
-      <c r="C36">
-        <v>264.94</v>
-      </c>
-      <c r="D36">
-        <v>229.74</v>
-      </c>
-      <c r="E36">
-        <v>245.14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
       <c r="B37">
-        <v>230.52</v>
+        <v>207</v>
       </c>
       <c r="C37">
-        <v>292.2</v>
+        <v>207</v>
       </c>
       <c r="D37">
-        <v>239.32</v>
+        <v>207</v>
       </c>
       <c r="E37">
-        <v>270.2</v>
+        <v>207</v>
+      </c>
+      <c r="F37">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="7">
+        <v>15.304355133142501</v>
+      </c>
+      <c r="C38" s="8">
+        <v>74.014850873205901</v>
+      </c>
+      <c r="D38" s="8">
+        <v>26.8690772260742</v>
+      </c>
+      <c r="E38" s="7">
+        <v>24.278765187454798</v>
+      </c>
+      <c r="F38">
+        <v>59.382697696635397</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="8">
+        <v>27.885802356612501</v>
+      </c>
+      <c r="C39" s="8">
+        <v>99.446653621520994</v>
+      </c>
+      <c r="D39" s="8">
+        <v>40.227680033444599</v>
+      </c>
+      <c r="E39" s="7">
+        <v>18.397699324604002</v>
+      </c>
+      <c r="F39">
+        <v>72.741300504005693</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="7">
+        <v>14.5240261890238</v>
+      </c>
+      <c r="C40" s="8">
+        <v>133.471594355462</v>
+      </c>
+      <c r="D40" s="8">
+        <v>35.9097541772189</v>
+      </c>
+      <c r="E40" s="7">
+        <v>57.588434738181697</v>
+      </c>
+      <c r="F40">
+        <v>73.1746545948875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>